<commit_message>
Add max root depth msmts
</commit_message>
<xml_diff>
--- a/data-raw/_raw/vn/2019/rd_20190626-phen.xlsx
+++ b/data-raw/_raw/vn/2019/rd_20190626-phen.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vnichols\Box Sync\1_Gina_Projects\proj_Marsden\_theme-2019data\_data\raw_entered\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vnichols\Box Sync\1_Gina_Projects\proj_Marsden\_theme-2019data\_data\raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="15">
   <si>
     <t>date</t>
   </si>
@@ -64,7 +64,16 @@
     <t>Leaf area not exposed to light is considered stem. Done on Matt's machine.</t>
   </si>
   <si>
-    <t>stage_Vx</t>
+    <t>stage</t>
+  </si>
+  <si>
+    <t>V5</t>
+  </si>
+  <si>
+    <t>V4</t>
+  </si>
+  <si>
+    <t>plht_cm</t>
   </si>
 </sst>
 </file>
@@ -114,7 +123,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -181,6 +190,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -466,10 +481,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:P47"/>
+  <dimension ref="A1:Q47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+      <selection activeCell="E7" sqref="E7:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -477,45 +492,46 @@
     <col min="1" max="1" width="35.42578125" style="1" customWidth="1"/>
     <col min="2" max="3" width="12.140625" style="2" customWidth="1"/>
     <col min="4" max="4" width="8" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.85546875" style="3" customWidth="1"/>
-    <col min="7" max="7" width="12.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="9.140625" style="1"/>
-    <col min="17" max="17" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="16384" width="9.140625" style="1"/>
+    <col min="5" max="5" width="8" style="3" customWidth="1"/>
+    <col min="6" max="6" width="14.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.85546875" style="3" customWidth="1"/>
+    <col min="8" max="8" width="12.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.140625" style="1"/>
+    <col min="18" max="18" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="16" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="16" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="17" t="s">
         <v>10</v>
       </c>
       <c r="B4" s="17"/>
       <c r="C4" s="17"/>
       <c r="D4" s="17"/>
-      <c r="E4" s="17"/>
+      <c r="E4" s="24"/>
       <c r="F4" s="17"/>
       <c r="G4" s="17"/>
       <c r="H4" s="17"/>
@@ -526,8 +542,9 @@
       <c r="M4" s="17"/>
       <c r="N4" s="17"/>
       <c r="O4" s="17"/>
-    </row>
-    <row r="6" spans="1:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P4" s="17"/>
+    </row>
+    <row r="6" spans="1:16" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>0</v>
       </c>
@@ -541,26 +558,29 @@
         <v>2</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="F6" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="G6" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="G6" s="9" t="s">
+      <c r="H6" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="H6" s="9" t="s">
+      <c r="I6" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="I6" s="9"/>
       <c r="J6" s="9"/>
       <c r="K6" s="9"/>
-      <c r="L6" s="7"/>
+      <c r="L6" s="9"/>
       <c r="M6" s="7"/>
       <c r="N6" s="7"/>
       <c r="O6" s="7"/>
-    </row>
-    <row r="7" spans="1:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P6" s="7"/>
+    </row>
+    <row r="7" spans="1:16" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="10">
         <v>43642</v>
       </c>
@@ -573,81 +593,84 @@
       <c r="D7" s="11">
         <v>1</v>
       </c>
-      <c r="E7" s="18">
+      <c r="E7" s="25"/>
+      <c r="F7" s="18">
         <v>3.5</v>
       </c>
-      <c r="F7" s="18">
-        <v>5</v>
-      </c>
-      <c r="G7" s="18">
-        <v>5</v>
-      </c>
-      <c r="H7" s="21">
-        <v>5</v>
-      </c>
-      <c r="I7" s="12"/>
+      <c r="G7" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="H7" s="18">
+        <v>5</v>
+      </c>
+      <c r="I7" s="21">
+        <v>5</v>
+      </c>
       <c r="J7" s="12"/>
       <c r="K7" s="12"/>
       <c r="L7" s="12"/>
       <c r="M7" s="12"/>
       <c r="N7" s="12"/>
       <c r="O7" s="12"/>
-    </row>
-    <row r="8" spans="1:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P7" s="12"/>
+    </row>
+    <row r="8" spans="1:16" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="10"/>
       <c r="B8" s="11"/>
       <c r="C8" s="11"/>
       <c r="D8" s="11">
         <v>2</v>
       </c>
-      <c r="E8" s="18">
+      <c r="E8" s="25"/>
+      <c r="F8" s="18">
         <v>4</v>
       </c>
-      <c r="F8" s="18">
-        <v>5</v>
-      </c>
-      <c r="G8" s="18">
-        <v>5</v>
-      </c>
-      <c r="H8" s="21">
-        <v>5</v>
-      </c>
-      <c r="I8" s="12"/>
+      <c r="G8" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="H8" s="18">
+        <v>5</v>
+      </c>
+      <c r="I8" s="21">
+        <v>5</v>
+      </c>
       <c r="J8" s="12"/>
       <c r="K8" s="12"/>
       <c r="L8" s="12"/>
       <c r="M8" s="12"/>
       <c r="N8" s="12"/>
       <c r="O8" s="12"/>
-    </row>
-    <row r="9" spans="1:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P8" s="12"/>
+    </row>
+    <row r="9" spans="1:16" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="10"/>
       <c r="B9" s="11"/>
       <c r="C9" s="11"/>
       <c r="D9" s="11">
         <v>3</v>
       </c>
-      <c r="E9" s="18">
+      <c r="E9" s="25"/>
+      <c r="F9" s="18">
         <v>3.5</v>
       </c>
-      <c r="F9" s="18">
-        <v>5</v>
-      </c>
-      <c r="G9" s="18">
-        <v>5</v>
+      <c r="G9" s="18" t="s">
+        <v>12</v>
       </c>
       <c r="H9" s="18">
         <v>5</v>
       </c>
-      <c r="I9" s="12"/>
+      <c r="I9" s="18">
+        <v>5</v>
+      </c>
       <c r="J9" s="12"/>
       <c r="K9" s="12"/>
       <c r="L9" s="12"/>
       <c r="M9" s="12"/>
       <c r="N9" s="12"/>
       <c r="O9" s="12"/>
-    </row>
-    <row r="10" spans="1:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P9" s="12"/>
+    </row>
+    <row r="10" spans="1:16" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="10"/>
       <c r="B10" s="11">
         <v>12</v>
@@ -658,81 +681,81 @@
       <c r="D10" s="11">
         <v>1</v>
       </c>
-      <c r="E10" s="18">
+      <c r="F10" s="18">
         <v>3.75</v>
       </c>
-      <c r="F10" s="18">
-        <v>5</v>
-      </c>
-      <c r="G10" s="18">
-        <v>5</v>
+      <c r="G10" s="18" t="s">
+        <v>12</v>
       </c>
       <c r="H10" s="18">
         <v>5</v>
       </c>
-      <c r="I10" s="12"/>
+      <c r="I10" s="18">
+        <v>5</v>
+      </c>
       <c r="J10" s="12"/>
       <c r="K10" s="12"/>
       <c r="L10" s="12"/>
       <c r="M10" s="12"/>
       <c r="N10" s="12"/>
       <c r="O10" s="12"/>
-    </row>
-    <row r="11" spans="1:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P10" s="12"/>
+    </row>
+    <row r="11" spans="1:16" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="10"/>
       <c r="B11" s="11"/>
       <c r="C11" s="11"/>
       <c r="D11" s="11">
         <v>2</v>
       </c>
-      <c r="E11" s="18">
+      <c r="F11" s="18">
         <v>3.75</v>
       </c>
-      <c r="F11" s="18">
-        <v>4</v>
-      </c>
-      <c r="G11" s="18">
-        <v>4</v>
+      <c r="G11" s="18" t="s">
+        <v>13</v>
       </c>
       <c r="H11" s="18">
         <v>4</v>
       </c>
-      <c r="I11" s="12"/>
+      <c r="I11" s="18">
+        <v>4</v>
+      </c>
       <c r="J11" s="12"/>
       <c r="K11" s="12"/>
       <c r="L11" s="12"/>
       <c r="M11" s="12"/>
       <c r="N11" s="12"/>
       <c r="O11" s="12"/>
-    </row>
-    <row r="12" spans="1:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P11" s="12"/>
+    </row>
+    <row r="12" spans="1:16" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="10"/>
       <c r="B12" s="11"/>
       <c r="C12" s="11"/>
       <c r="D12" s="11">
         <v>3</v>
       </c>
-      <c r="E12" s="18">
+      <c r="F12" s="18">
         <v>4</v>
       </c>
-      <c r="F12" s="18">
-        <v>5</v>
-      </c>
-      <c r="G12" s="22">
-        <v>5</v>
-      </c>
-      <c r="H12" s="18">
-        <v>5</v>
-      </c>
-      <c r="I12" s="12"/>
+      <c r="G12" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="H12" s="22">
+        <v>5</v>
+      </c>
+      <c r="I12" s="18">
+        <v>5</v>
+      </c>
       <c r="J12" s="12"/>
       <c r="K12" s="12"/>
       <c r="L12" s="12"/>
       <c r="M12" s="12"/>
       <c r="N12" s="12"/>
       <c r="O12" s="12"/>
-    </row>
-    <row r="13" spans="1:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P12" s="12"/>
+    </row>
+    <row r="13" spans="1:16" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="10"/>
       <c r="B13" s="11">
         <v>35</v>
@@ -743,81 +766,84 @@
       <c r="D13" s="11">
         <v>1</v>
       </c>
-      <c r="E13" s="18">
+      <c r="E13" s="25"/>
+      <c r="F13" s="18">
         <v>3.25</v>
       </c>
-      <c r="F13" s="18">
+      <c r="G13" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="H13" s="22">
         <v>4</v>
       </c>
-      <c r="G13" s="22">
+      <c r="I13" s="18">
         <v>4</v>
       </c>
-      <c r="H13" s="18">
-        <v>4</v>
-      </c>
-      <c r="I13" s="12"/>
       <c r="J13" s="12"/>
       <c r="K13" s="12"/>
       <c r="L13" s="12"/>
       <c r="M13" s="12"/>
       <c r="N13" s="12"/>
       <c r="O13" s="12"/>
-    </row>
-    <row r="14" spans="1:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P13" s="12"/>
+    </row>
+    <row r="14" spans="1:16" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="10"/>
       <c r="B14" s="11"/>
       <c r="C14" s="11"/>
       <c r="D14" s="11">
         <v>2</v>
       </c>
-      <c r="E14" s="18">
+      <c r="E14" s="25"/>
+      <c r="F14" s="18">
         <v>3.5</v>
       </c>
-      <c r="F14" s="18">
-        <v>5</v>
-      </c>
-      <c r="G14" s="22">
-        <v>5</v>
-      </c>
-      <c r="H14" s="18">
-        <v>5</v>
-      </c>
-      <c r="I14" s="12"/>
+      <c r="G14" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="H14" s="22">
+        <v>5</v>
+      </c>
+      <c r="I14" s="18">
+        <v>5</v>
+      </c>
       <c r="J14" s="12"/>
       <c r="K14" s="12"/>
       <c r="L14" s="12"/>
       <c r="M14" s="12"/>
       <c r="N14" s="12"/>
       <c r="O14" s="12"/>
-    </row>
-    <row r="15" spans="1:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P14" s="12"/>
+    </row>
+    <row r="15" spans="1:16" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="10"/>
       <c r="B15" s="11"/>
       <c r="C15" s="11"/>
       <c r="D15" s="11">
         <v>3</v>
       </c>
-      <c r="E15" s="18">
+      <c r="E15" s="25"/>
+      <c r="F15" s="18">
         <v>3.5</v>
       </c>
-      <c r="F15" s="18">
+      <c r="G15" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="H15" s="22">
         <v>4</v>
       </c>
-      <c r="G15" s="22">
+      <c r="I15" s="18">
         <v>4</v>
       </c>
-      <c r="H15" s="18">
-        <v>4</v>
-      </c>
-      <c r="I15" s="12"/>
       <c r="J15" s="12"/>
       <c r="K15" s="12"/>
       <c r="L15" s="12"/>
       <c r="M15" s="12"/>
       <c r="N15" s="12"/>
       <c r="O15" s="12"/>
-    </row>
-    <row r="16" spans="1:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P15" s="12"/>
+    </row>
+    <row r="16" spans="1:16" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="10"/>
       <c r="B16" s="11">
         <v>19</v>
@@ -828,81 +854,84 @@
       <c r="D16" s="11">
         <v>1</v>
       </c>
-      <c r="E16" s="18">
+      <c r="E16" s="25"/>
+      <c r="F16" s="18">
         <v>3.5</v>
       </c>
-      <c r="F16" s="18">
+      <c r="G16" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="H16" s="22">
         <v>4</v>
       </c>
-      <c r="G16" s="22">
+      <c r="I16" s="18">
         <v>4</v>
       </c>
-      <c r="H16" s="18">
-        <v>4</v>
-      </c>
-      <c r="I16" s="12"/>
       <c r="J16" s="12"/>
       <c r="K16" s="12"/>
       <c r="L16" s="12"/>
       <c r="M16" s="12"/>
       <c r="N16" s="12"/>
       <c r="O16" s="12"/>
-    </row>
-    <row r="17" spans="1:16" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P16" s="12"/>
+    </row>
+    <row r="17" spans="1:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="10"/>
       <c r="B17" s="11"/>
       <c r="C17" s="11"/>
       <c r="D17" s="11">
         <v>2</v>
       </c>
-      <c r="E17" s="18">
+      <c r="E17" s="25"/>
+      <c r="F17" s="18">
         <v>4.25</v>
       </c>
-      <c r="F17" s="18">
-        <v>5</v>
-      </c>
-      <c r="G17" s="22">
-        <v>5</v>
-      </c>
-      <c r="H17" s="18">
-        <v>5</v>
-      </c>
-      <c r="I17" s="12"/>
+      <c r="G17" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="H17" s="22">
+        <v>5</v>
+      </c>
+      <c r="I17" s="18">
+        <v>5</v>
+      </c>
       <c r="J17" s="12"/>
       <c r="K17" s="12"/>
       <c r="L17" s="12"/>
       <c r="M17" s="12"/>
       <c r="N17" s="12"/>
       <c r="O17" s="12"/>
-    </row>
-    <row r="18" spans="1:16" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P17" s="12"/>
+    </row>
+    <row r="18" spans="1:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="10"/>
       <c r="B18" s="11"/>
       <c r="C18" s="11"/>
       <c r="D18" s="11">
         <v>3</v>
       </c>
-      <c r="E18" s="18">
+      <c r="E18" s="25"/>
+      <c r="F18" s="18">
         <v>3.5</v>
       </c>
-      <c r="F18" s="18">
-        <v>5</v>
-      </c>
-      <c r="G18" s="22">
-        <v>5</v>
-      </c>
-      <c r="H18" s="18">
-        <v>5</v>
-      </c>
-      <c r="I18" s="12"/>
+      <c r="G18" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="H18" s="22">
+        <v>5</v>
+      </c>
+      <c r="I18" s="18">
+        <v>5</v>
+      </c>
       <c r="J18" s="12"/>
       <c r="K18" s="12"/>
       <c r="L18" s="12"/>
       <c r="M18" s="12"/>
       <c r="N18" s="12"/>
       <c r="O18" s="12"/>
-    </row>
-    <row r="19" spans="1:16" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P18" s="12"/>
+    </row>
+    <row r="19" spans="1:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="10"/>
       <c r="B19" s="11">
         <v>21</v>
@@ -913,79 +942,82 @@
       <c r="D19" s="11">
         <v>1</v>
       </c>
-      <c r="E19" s="18">
+      <c r="E19" s="25"/>
+      <c r="F19" s="18">
         <v>4.25</v>
       </c>
-      <c r="F19" s="18">
-        <v>5</v>
-      </c>
-      <c r="G19" s="22">
-        <v>5</v>
-      </c>
-      <c r="H19" s="18">
-        <v>5</v>
-      </c>
-      <c r="I19" s="12"/>
+      <c r="G19" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="H19" s="22">
+        <v>5</v>
+      </c>
+      <c r="I19" s="18">
+        <v>5</v>
+      </c>
       <c r="J19" s="12"/>
       <c r="K19" s="12"/>
       <c r="L19" s="12"/>
       <c r="M19" s="12"/>
       <c r="N19" s="12"/>
       <c r="O19" s="12"/>
-    </row>
-    <row r="20" spans="1:16" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P19" s="12"/>
+    </row>
+    <row r="20" spans="1:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="13"/>
       <c r="B20" s="14"/>
       <c r="C20" s="14"/>
       <c r="D20" s="11">
         <v>2</v>
       </c>
-      <c r="E20" s="19">
+      <c r="E20" s="25"/>
+      <c r="F20" s="19">
         <v>3.75</v>
       </c>
-      <c r="F20" s="19">
-        <v>5</v>
-      </c>
-      <c r="G20" s="20">
-        <v>5</v>
+      <c r="G20" s="18" t="s">
+        <v>12</v>
       </c>
       <c r="H20" s="20">
         <v>5</v>
       </c>
-      <c r="J20" s="15"/>
+      <c r="I20" s="20">
+        <v>5</v>
+      </c>
       <c r="K20" s="15"/>
-      <c r="M20" s="15"/>
+      <c r="L20" s="15"/>
       <c r="N20" s="15"/>
       <c r="O20" s="15"/>
       <c r="P20" s="15"/>
-    </row>
-    <row r="21" spans="1:16" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q20" s="15"/>
+    </row>
+    <row r="21" spans="1:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="13"/>
       <c r="B21" s="14"/>
       <c r="C21" s="14"/>
       <c r="D21" s="11">
         <v>3</v>
       </c>
-      <c r="E21" s="19">
+      <c r="E21" s="25"/>
+      <c r="F21" s="19">
         <v>4.5</v>
       </c>
-      <c r="F21" s="19">
-        <v>5</v>
-      </c>
-      <c r="G21" s="20">
-        <v>5</v>
+      <c r="G21" s="18" t="s">
+        <v>12</v>
       </c>
       <c r="H21" s="20">
         <v>5</v>
       </c>
-      <c r="J21" s="15"/>
+      <c r="I21" s="20">
+        <v>5</v>
+      </c>
       <c r="K21" s="15"/>
-      <c r="M21" s="15"/>
+      <c r="L21" s="15"/>
       <c r="N21" s="15"/>
       <c r="O21" s="15"/>
       <c r="P21" s="15"/>
-    </row>
-    <row r="22" spans="1:16" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q21" s="15"/>
+    </row>
+    <row r="22" spans="1:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="13"/>
       <c r="B22" s="14">
         <v>43</v>
@@ -996,78 +1028,81 @@
       <c r="D22" s="11">
         <v>1</v>
       </c>
-      <c r="E22" s="19">
+      <c r="E22" s="25"/>
+      <c r="F22" s="19">
         <v>4.5</v>
       </c>
-      <c r="F22" s="19">
-        <v>5</v>
-      </c>
-      <c r="G22" s="20">
-        <v>5</v>
+      <c r="G22" s="18" t="s">
+        <v>12</v>
       </c>
       <c r="H22" s="20">
         <v>5</v>
       </c>
-      <c r="J22" s="15"/>
+      <c r="I22" s="20">
+        <v>5</v>
+      </c>
       <c r="K22" s="15"/>
-      <c r="M22" s="15"/>
+      <c r="L22" s="15"/>
       <c r="N22" s="15"/>
       <c r="O22" s="15"/>
       <c r="P22" s="15"/>
-    </row>
-    <row r="23" spans="1:16" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q22" s="15"/>
+    </row>
+    <row r="23" spans="1:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="13"/>
       <c r="B23" s="14"/>
       <c r="C23" s="14"/>
       <c r="D23" s="11">
         <v>2</v>
       </c>
-      <c r="E23" s="19">
+      <c r="E23" s="25"/>
+      <c r="F23" s="19">
         <v>4.25</v>
       </c>
-      <c r="F23" s="19">
-        <v>5</v>
-      </c>
-      <c r="G23" s="20">
-        <v>5</v>
+      <c r="G23" s="18" t="s">
+        <v>12</v>
       </c>
       <c r="H23" s="20">
         <v>5</v>
       </c>
-      <c r="J23" s="15"/>
+      <c r="I23" s="20">
+        <v>5</v>
+      </c>
       <c r="K23" s="15"/>
-      <c r="M23" s="15"/>
+      <c r="L23" s="15"/>
       <c r="N23" s="15"/>
       <c r="O23" s="15"/>
       <c r="P23" s="15"/>
-    </row>
-    <row r="24" spans="1:16" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q23" s="15"/>
+    </row>
+    <row r="24" spans="1:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="13"/>
       <c r="B24" s="14"/>
       <c r="C24" s="14"/>
       <c r="D24" s="11">
         <v>3</v>
       </c>
-      <c r="E24" s="19">
+      <c r="E24" s="25"/>
+      <c r="F24" s="19">
         <v>3.5</v>
       </c>
-      <c r="F24" s="19">
-        <v>5</v>
-      </c>
-      <c r="G24" s="20">
-        <v>5</v>
+      <c r="G24" s="18" t="s">
+        <v>12</v>
       </c>
       <c r="H24" s="20">
+        <v>5</v>
+      </c>
+      <c r="I24" s="20">
         <v>4</v>
       </c>
-      <c r="J24" s="15"/>
       <c r="K24" s="15"/>
-      <c r="M24" s="15"/>
+      <c r="L24" s="15"/>
       <c r="N24" s="15"/>
       <c r="O24" s="15"/>
       <c r="P24" s="15"/>
-    </row>
-    <row r="25" spans="1:16" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q24" s="15"/>
+    </row>
+    <row r="25" spans="1:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="13"/>
       <c r="B25" s="14">
         <v>45</v>
@@ -1078,78 +1113,81 @@
       <c r="D25" s="11">
         <v>1</v>
       </c>
-      <c r="E25" s="19">
+      <c r="E25" s="25"/>
+      <c r="F25" s="19">
         <v>3.25</v>
       </c>
-      <c r="F25" s="19">
-        <v>5</v>
-      </c>
-      <c r="G25" s="20">
-        <v>5</v>
+      <c r="G25" s="18" t="s">
+        <v>12</v>
       </c>
       <c r="H25" s="20">
         <v>5</v>
       </c>
-      <c r="J25" s="15"/>
+      <c r="I25" s="20">
+        <v>5</v>
+      </c>
       <c r="K25" s="15"/>
-      <c r="M25" s="15"/>
+      <c r="L25" s="15"/>
       <c r="N25" s="15"/>
       <c r="O25" s="15"/>
       <c r="P25" s="15"/>
-    </row>
-    <row r="26" spans="1:16" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q25" s="15"/>
+    </row>
+    <row r="26" spans="1:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="13"/>
       <c r="B26" s="14"/>
       <c r="C26" s="14"/>
       <c r="D26" s="11">
         <v>2</v>
       </c>
-      <c r="E26" s="19">
+      <c r="E26" s="25"/>
+      <c r="F26" s="19">
         <v>4.5</v>
       </c>
-      <c r="F26" s="19">
-        <v>5</v>
-      </c>
-      <c r="G26" s="20">
-        <v>5</v>
+      <c r="G26" s="18" t="s">
+        <v>12</v>
       </c>
       <c r="H26" s="20">
         <v>5</v>
       </c>
-      <c r="J26" s="15"/>
+      <c r="I26" s="20">
+        <v>5</v>
+      </c>
       <c r="K26" s="15"/>
-      <c r="M26" s="15"/>
+      <c r="L26" s="15"/>
       <c r="N26" s="15"/>
       <c r="O26" s="15"/>
       <c r="P26" s="15"/>
-    </row>
-    <row r="27" spans="1:16" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q26" s="15"/>
+    </row>
+    <row r="27" spans="1:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="13"/>
       <c r="B27" s="14"/>
       <c r="C27" s="14"/>
       <c r="D27" s="11">
         <v>3</v>
       </c>
-      <c r="E27" s="19">
+      <c r="E27" s="25"/>
+      <c r="F27" s="19">
         <v>4.25</v>
       </c>
-      <c r="F27" s="19">
-        <v>5</v>
-      </c>
-      <c r="G27" s="20">
-        <v>5</v>
+      <c r="G27" s="18" t="s">
+        <v>12</v>
       </c>
       <c r="H27" s="20">
         <v>5</v>
       </c>
-      <c r="J27" s="15"/>
+      <c r="I27" s="20">
+        <v>5</v>
+      </c>
       <c r="K27" s="15"/>
-      <c r="M27" s="15"/>
+      <c r="L27" s="15"/>
       <c r="N27" s="15"/>
       <c r="O27" s="15"/>
       <c r="P27" s="15"/>
-    </row>
-    <row r="28" spans="1:16" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Q27" s="15"/>
+    </row>
+    <row r="28" spans="1:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
       <c r="B28" s="5">
         <v>27</v>
@@ -1160,60 +1198,63 @@
       <c r="D28" s="11">
         <v>1</v>
       </c>
-      <c r="E28" s="20">
+      <c r="E28" s="25"/>
+      <c r="F28" s="20">
         <v>4.75</v>
       </c>
-      <c r="F28" s="20">
-        <v>5</v>
-      </c>
-      <c r="G28" s="20">
-        <v>5</v>
-      </c>
-      <c r="H28" s="23">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="29" spans="1:16" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G28" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="H28" s="20">
+        <v>5</v>
+      </c>
+      <c r="I28" s="23">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
       <c r="D29" s="11">
         <v>2</v>
       </c>
-      <c r="E29" s="20">
+      <c r="E29" s="25"/>
+      <c r="F29" s="20">
         <v>4.25</v>
       </c>
-      <c r="F29" s="20">
-        <v>5</v>
-      </c>
-      <c r="G29" s="20">
-        <v>5</v>
-      </c>
-      <c r="H29" s="23">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="30" spans="1:16" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G29" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="H29" s="20">
+        <v>5</v>
+      </c>
+      <c r="I29" s="23">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="4"/>
       <c r="B30" s="5"/>
       <c r="C30" s="5"/>
       <c r="D30" s="11">
         <v>3</v>
       </c>
-      <c r="E30" s="20">
+      <c r="E30" s="25"/>
+      <c r="F30" s="20">
         <v>4.5</v>
       </c>
-      <c r="F30" s="20">
-        <v>5</v>
-      </c>
-      <c r="G30" s="20">
-        <v>5</v>
-      </c>
-      <c r="H30" s="23">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="31" spans="1:16" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G30" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="H30" s="20">
+        <v>5</v>
+      </c>
+      <c r="I30" s="23">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="4"/>
       <c r="B31" s="5"/>
       <c r="C31" s="5"/>
@@ -1221,8 +1262,9 @@
       <c r="E31" s="6"/>
       <c r="F31" s="6"/>
       <c r="G31" s="6"/>
-    </row>
-    <row r="32" spans="1:16" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H31" s="6"/>
+    </row>
+    <row r="32" spans="1:17" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="4"/>
       <c r="B32" s="5"/>
       <c r="C32" s="5"/>
@@ -1230,8 +1272,9 @@
       <c r="E32" s="6"/>
       <c r="F32" s="6"/>
       <c r="G32" s="6"/>
-    </row>
-    <row r="33" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H32" s="6"/>
+    </row>
+    <row r="33" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="4"/>
       <c r="B33" s="5"/>
       <c r="C33" s="5"/>
@@ -1239,8 +1282,9 @@
       <c r="E33" s="6"/>
       <c r="F33" s="6"/>
       <c r="G33" s="6"/>
-    </row>
-    <row r="34" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H33" s="6"/>
+    </row>
+    <row r="34" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="4"/>
       <c r="B34" s="5"/>
       <c r="C34" s="5"/>
@@ -1248,8 +1292,9 @@
       <c r="E34" s="6"/>
       <c r="F34" s="6"/>
       <c r="G34" s="6"/>
-    </row>
-    <row r="35" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H34" s="6"/>
+    </row>
+    <row r="35" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="4"/>
       <c r="B35" s="5"/>
       <c r="C35" s="5"/>
@@ -1257,8 +1302,9 @@
       <c r="E35" s="6"/>
       <c r="F35" s="6"/>
       <c r="G35" s="6"/>
-    </row>
-    <row r="36" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H35" s="6"/>
+    </row>
+    <row r="36" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="4"/>
       <c r="B36" s="5"/>
       <c r="C36" s="5"/>
@@ -1266,8 +1312,9 @@
       <c r="E36" s="6"/>
       <c r="F36" s="6"/>
       <c r="G36" s="6"/>
-    </row>
-    <row r="37" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H36" s="6"/>
+    </row>
+    <row r="37" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="4"/>
       <c r="B37" s="5"/>
       <c r="C37" s="5"/>
@@ -1275,8 +1322,9 @@
       <c r="E37" s="6"/>
       <c r="F37" s="6"/>
       <c r="G37" s="6"/>
-    </row>
-    <row r="38" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H37" s="6"/>
+    </row>
+    <row r="38" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="4"/>
       <c r="B38" s="5"/>
       <c r="C38" s="5"/>
@@ -1284,8 +1332,9 @@
       <c r="E38" s="6"/>
       <c r="F38" s="6"/>
       <c r="G38" s="6"/>
-    </row>
-    <row r="39" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H38" s="6"/>
+    </row>
+    <row r="39" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="4"/>
       <c r="B39" s="5"/>
       <c r="C39" s="5"/>
@@ -1293,8 +1342,9 @@
       <c r="E39" s="6"/>
       <c r="F39" s="6"/>
       <c r="G39" s="6"/>
-    </row>
-    <row r="40" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H39" s="6"/>
+    </row>
+    <row r="40" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="4"/>
       <c r="B40" s="5"/>
       <c r="C40" s="5"/>
@@ -1302,8 +1352,9 @@
       <c r="E40" s="6"/>
       <c r="F40" s="6"/>
       <c r="G40" s="6"/>
-    </row>
-    <row r="41" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H40" s="6"/>
+    </row>
+    <row r="41" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="4"/>
       <c r="B41" s="5"/>
       <c r="C41" s="5"/>
@@ -1311,8 +1362,9 @@
       <c r="E41" s="6"/>
       <c r="F41" s="6"/>
       <c r="G41" s="6"/>
-    </row>
-    <row r="42" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H41" s="6"/>
+    </row>
+    <row r="42" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="4"/>
       <c r="B42" s="5"/>
       <c r="C42" s="5"/>
@@ -1320,8 +1372,9 @@
       <c r="E42" s="6"/>
       <c r="F42" s="6"/>
       <c r="G42" s="6"/>
-    </row>
-    <row r="43" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H42" s="6"/>
+    </row>
+    <row r="43" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="4"/>
       <c r="B43" s="5"/>
       <c r="C43" s="5"/>
@@ -1329,8 +1382,9 @@
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-    </row>
-    <row r="44" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H43" s="6"/>
+    </row>
+    <row r="44" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="4"/>
       <c r="B44" s="5"/>
       <c r="C44" s="5"/>
@@ -1338,8 +1392,9 @@
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-    </row>
-    <row r="45" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H44" s="6"/>
+    </row>
+    <row r="45" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="4"/>
       <c r="B45" s="5"/>
       <c r="C45" s="5"/>
@@ -1347,8 +1402,9 @@
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-    </row>
-    <row r="46" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H45" s="6"/>
+    </row>
+    <row r="46" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="4"/>
       <c r="B46" s="5"/>
       <c r="C46" s="5"/>
@@ -1356,8 +1412,9 @@
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-    </row>
-    <row r="47" spans="1:7" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H46" s="6"/>
+    </row>
+    <row r="47" spans="1:8" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="4"/>
       <c r="B47" s="5"/>
       <c r="C47" s="5"/>
@@ -1365,6 +1422,7 @@
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
+      <c r="H47" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>